<commit_message>
Añadido nuevo fichero excel
</commit_message>
<xml_diff>
--- a/Screenshots/_Screenshots.xlsx
+++ b/Screenshots/_Screenshots.xlsx
@@ -12,8 +12,9 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_Screenshots" localSheetId="0">Hoja1!$B$3:$G$140</definedName>
     <definedName name="new_1" localSheetId="0">Hoja1!#REF!</definedName>
-    <definedName name="tmp" localSheetId="0">Hoja1!$B$3:$G$85</definedName>
+    <definedName name="tmp" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -21,7 +22,19 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="new 1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="1" name="_Screenshots" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\_PELAYO\Software\Eclipse Neon\workspace\markets_data\Screenshots\_Screenshots.txt" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="6">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="new 1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\new 1.txt" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="6">
         <textField type="text"/>
@@ -33,7 +46,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="tmp" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="3" name="tmp" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\tmp.txt" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="6">
         <textField/>
@@ -49,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="344">
   <si>
     <t>Salud</t>
   </si>
@@ -709,6 +722,378 @@
   </si>
   <si>
     <t>Rentabilidad Dividendo</t>
+  </si>
+  <si>
+    <t>AENA SME S.A. (AENA)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/aena-aeropuertos-sa</t>
+  </si>
+  <si>
+    <t>Allianz SE VNA O.N. (ALVG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/allianz-ag</t>
+  </si>
+  <si>
+    <t>Atlantia SpA (ATL)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/atlantia</t>
+  </si>
+  <si>
+    <t>Aeroespacial y defensa</t>
+  </si>
+  <si>
+    <t>BAE Systems PLC (BAES)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/bae-systems</t>
+  </si>
+  <si>
+    <t>Principales medicamentos</t>
+  </si>
+  <si>
+    <t>Bayer AG NA (BAYGn)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/bayer-ag</t>
+  </si>
+  <si>
+    <t>BCE Inc. (BCE)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/bce</t>
+  </si>
+  <si>
+    <t>Bellway PLC (BWY)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/bellway</t>
+  </si>
+  <si>
+    <t>Bouygues SA (BOUY)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/bouygues</t>
+  </si>
+  <si>
+    <t>Brookfield Infrastructure Partners LP (BIP_u)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/brookfield-infrastructure-partners</t>
+  </si>
+  <si>
+    <t>Cardinal Health Inc (CAH)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/cardinal-health</t>
+  </si>
+  <si>
+    <t>Actividades recreativas</t>
+  </si>
+  <si>
+    <t>Carnival Corporation (CCL)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/carnival-corp-exch</t>
+  </si>
+  <si>
+    <t>Chevron Corp (CVX)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/chevron</t>
+  </si>
+  <si>
+    <t>Close Brothers Group plc (CBRO)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/close-brothers</t>
+  </si>
+  <si>
+    <t>CNP Assurances SA (CNPP)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/cnp-assurances</t>
+  </si>
+  <si>
+    <t>Dominion Resources Inc (D)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/dominion-res</t>
+  </si>
+  <si>
+    <t>Papel y productos derivados</t>
+  </si>
+  <si>
+    <t>DS Smith PLC (SMDS)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/ds-smith</t>
+  </si>
+  <si>
+    <t>Deutsche Telekom AG Na (DTEGn)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/dt-telekom</t>
+  </si>
+  <si>
+    <t>E.ON SE NA (EONGn)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/e.on</t>
+  </si>
+  <si>
+    <t>ERG (ERG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/erg-spa</t>
+  </si>
+  <si>
+    <t>Naturgy Energy Group S.A. (NTGY)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/gas-natural-sdg</t>
+  </si>
+  <si>
+    <t>Engie SA (ENGIE)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/gdf-suez</t>
+  </si>
+  <si>
+    <t>Gilead Sciences Inc (GILD)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/gilead-sciences-inc</t>
+  </si>
+  <si>
+    <t>GlaxoSmithKline PLC (GSK)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/glaxosmithkline</t>
+  </si>
+  <si>
+    <t>Servicios personales</t>
+  </si>
+  <si>
+    <t>H&amp;R Block Inc (HRB)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/h---r-block-inc</t>
+  </si>
+  <si>
+    <t>Hanesbrands Inc (HBI)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/hanesbrands</t>
+  </si>
+  <si>
+    <t>Productos recreativos</t>
+  </si>
+  <si>
+    <t>Harley-Davidson Inc (HOG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/harley-davidson</t>
+  </si>
+  <si>
+    <t>HCP Inc (HCP)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/hcp-inc</t>
+  </si>
+  <si>
+    <t>Servicios informáticos</t>
+  </si>
+  <si>
+    <t>International Business Machines (IBM)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/ibm</t>
+  </si>
+  <si>
+    <t>Comercio minoristas (especializado)</t>
+  </si>
+  <si>
+    <t>Inchcape PLC (INCH)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/inchcape</t>
+  </si>
+  <si>
+    <t>Kinder Morgan Inc (KMI)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/kinder-morgan</t>
+  </si>
+  <si>
+    <t>Maquinaria agrícola y de construcción</t>
+  </si>
+  <si>
+    <t>Konecranes ABP (KCRA)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/konecranes</t>
+  </si>
+  <si>
+    <t>Muebles y accesorios</t>
+  </si>
+  <si>
+    <t>Leggett &amp; Platt Incorporated (LEG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/leggett---platt</t>
+  </si>
+  <si>
+    <t>LTC Properties Inc (LTC)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/ltc-properties-inc</t>
+  </si>
+  <si>
+    <t>Mercury General Corporation (MCY)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/mercury-general-corp</t>
+  </si>
+  <si>
+    <t>Bebidas (alcohólicas)</t>
+  </si>
+  <si>
+    <t>Molson Coors Brewing Co Class B (TAP)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/molson-coors</t>
+  </si>
+  <si>
+    <t>Contenedores y empaquetado</t>
+  </si>
+  <si>
+    <t>Mondi PLC (MNDI)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/mond</t>
+  </si>
+  <si>
+    <t>Munich Re (MUVGn)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/muench.-rueck</t>
+  </si>
+  <si>
+    <t>National Fuel Gas Company (NFG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/national-fuel-gas-comp</t>
+  </si>
+  <si>
+    <t>People’s United Financial Inc (PBCT)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/peoples-united-financial</t>
+  </si>
+  <si>
+    <t>Pfizer Inc (PFE)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/pfizer</t>
+  </si>
+  <si>
+    <t>Seguros (accidentes y salud)</t>
+  </si>
+  <si>
+    <t>Principal Financial Group Inc (PFG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/principal-fin</t>
+  </si>
+  <si>
+    <t>Prudential Financial Inc (PRU)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/prudential-fin</t>
+  </si>
+  <si>
+    <t>Camiones</t>
+  </si>
+  <si>
+    <t>Royal Mail PLC (RMG)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/royal-mail</t>
+  </si>
+  <si>
+    <t>SCOR SE (SCOR)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/scor</t>
+  </si>
+  <si>
+    <t>Bank of Nova Scotia (BNS)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/scotiabank</t>
+  </si>
+  <si>
+    <t>Southern Company (SO)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/southern-co</t>
+  </si>
+  <si>
+    <t>Suez SA (SEVI)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/suez-environnement-s.a.</t>
+  </si>
+  <si>
+    <t>Suncor Energy Inc (SU)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/suncor-energy-inc.</t>
+  </si>
+  <si>
+    <t>Tate &amp; Lyle PLC (TATE)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/tate---lyle</t>
+  </si>
+  <si>
+    <t>Toronto Dominion Bank (TD)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/toronto-dominion-bank</t>
+  </si>
+  <si>
+    <t>Valero Energy Corporation (VLO)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/valero-energy</t>
+  </si>
+  <si>
+    <t>Ventas Inc (VTR)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/ventas-inc</t>
+  </si>
+  <si>
+    <t>Verizon Communications Inc (VZ)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/verizon-communications</t>
+  </si>
+  <si>
+    <t>W P Carey Inc (WPC)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/w-p-carey-inc</t>
+  </si>
+  <si>
+    <t>Wells Fargo &amp; Company (WFC)</t>
+  </si>
+  <si>
+    <t>https://es.investing.com/equities/wells-fargo</t>
   </si>
 </sst>
 </file>
@@ -800,7 +1185,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="_Screenshots" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1090,18 +1475,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G85"/>
+  <dimension ref="B1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="61.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="54.42578125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -1128,182 +1513,182 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>13.85</v>
+        <v>5.84</v>
       </c>
       <c r="F3" s="3">
-        <v>3.98</v>
+        <v>110.1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>71</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3">
-        <v>12.12</v>
+        <v>5.46</v>
       </c>
       <c r="F4" s="3">
-        <v>17.73</v>
+        <v>11.06</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3">
-        <v>9.64</v>
+        <v>8.19</v>
       </c>
       <c r="F5" s="3">
-        <v>3.53</v>
+        <v>7.86</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
       <c r="E6" s="3">
-        <v>9.52</v>
+        <v>4.28</v>
       </c>
       <c r="F6" s="3">
-        <v>19.25</v>
+        <v>25.16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>92</v>
+        <v>222</v>
       </c>
       <c r="E7" s="3">
-        <v>9.2799999999999994</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="F7" s="3">
-        <v>2.0699999999999998</v>
+        <v>88.9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>93</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="E8" s="3">
-        <v>8.6199999999999992</v>
+        <v>7.91</v>
       </c>
       <c r="F8" s="3">
-        <v>17.63</v>
+        <v>80.290000000000006</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3">
-        <v>8.34</v>
+        <v>5.51</v>
       </c>
       <c r="F9" s="3">
-        <v>27.02</v>
+        <v>273.43</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>146</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>208</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>209</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="E10" s="3">
-        <v>8.2799999999999994</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="F10" s="3">
-        <v>18.02</v>
+        <v>17.62</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3">
         <v>8.07</v>
       </c>
       <c r="F11" s="3">
-        <v>78.459999999999994</v>
+        <v>15.25</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
@@ -1314,36 +1699,36 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3">
-        <v>8.06</v>
+        <v>5.54</v>
       </c>
       <c r="F12" s="3">
-        <v>7.5</v>
+        <v>55</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>227</v>
       </c>
       <c r="E13" s="3">
-        <v>8</v>
+        <v>4.07</v>
       </c>
       <c r="F13" s="3">
-        <v>14.74</v>
+        <v>17.66</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>24</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
@@ -1351,239 +1736,239 @@
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3">
-        <v>8</v>
+        <v>5.77</v>
       </c>
       <c r="F14" s="3">
-        <v>6.38</v>
+        <v>30.3</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="E15" s="3">
-        <v>7.76</v>
+        <v>6.62</v>
       </c>
       <c r="F15" s="3">
-        <v>12.95</v>
+        <v>59.52</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>178</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>157</v>
+        <v>322</v>
       </c>
       <c r="E16" s="3">
-        <v>7.66</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="F16" s="3">
-        <v>8</v>
+        <v>91.3</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>158</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3">
-        <v>7.47</v>
+        <v>6.66</v>
       </c>
       <c r="F17" s="3">
-        <v>3.25</v>
+        <v>5.26</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="E18" s="3">
-        <v>7.41</v>
+        <v>5.29</v>
       </c>
       <c r="F18" s="3">
-        <v>4.01</v>
+        <v>5.3</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="E19" s="3">
-        <v>7.26</v>
+        <v>5.31</v>
       </c>
       <c r="F19" s="3">
-        <v>4.9000000000000004</v>
+        <v>58.48</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="E20" s="3">
-        <v>7.21</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="F20" s="3">
-        <v>6.37</v>
+        <v>59.71</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>66</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3">
-        <v>7.19</v>
+        <v>5.44</v>
       </c>
       <c r="F21" s="3">
-        <v>64.2</v>
+        <v>42.14</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>161</v>
+        <v>232</v>
       </c>
       <c r="E22" s="3">
-        <v>7.04</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F22" s="3">
-        <v>14.75</v>
+        <v>58.56</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>162</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="E23" s="3">
-        <v>7.01</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="F23" s="3">
-        <v>14.05</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>123</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="E24" s="3">
-        <v>6.98</v>
+        <v>6.33</v>
       </c>
       <c r="F24" s="3">
-        <v>8.9</v>
+        <v>85.69</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>236</v>
       </c>
       <c r="E25" s="3">
-        <v>6.85</v>
+        <v>4.49</v>
       </c>
       <c r="F25" s="3">
-        <v>47.27</v>
+        <v>14.13</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>75</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1591,159 +1976,159 @@
         <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="E26" s="3">
-        <v>6.81</v>
+        <v>6.36</v>
       </c>
       <c r="F26" s="3">
-        <v>30.45</v>
+        <v>102.5</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>212</v>
+        <v>52</v>
       </c>
       <c r="E27" s="3">
-        <v>6.8</v>
+        <v>7.2</v>
       </c>
       <c r="F27" s="3">
-        <v>2.64</v>
+        <v>63.39</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>213</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>208</v>
+        <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>210</v>
+        <v>54</v>
       </c>
       <c r="E28" s="3">
-        <v>6.78</v>
+        <v>5.77</v>
       </c>
       <c r="F28" s="3">
-        <v>27.62</v>
+        <v>5.19</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="E29" s="3">
-        <v>6.7</v>
+        <v>4.08</v>
       </c>
       <c r="F29" s="3">
-        <v>39.14</v>
+        <v>2.62</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="E30" s="3">
-        <v>6.66</v>
+        <v>5.76</v>
       </c>
       <c r="F30" s="3">
-        <v>5.04</v>
+        <v>5.49</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>179</v>
+        <v>61</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>180</v>
+        <v>62</v>
       </c>
       <c r="E31" s="3">
-        <v>6.65</v>
+        <v>8.65</v>
       </c>
       <c r="F31" s="3">
-        <v>2.21</v>
+        <v>18.73</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>181</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E32" s="3">
-        <v>6.62</v>
+        <v>7.21</v>
       </c>
       <c r="F32" s="3">
-        <v>57.49</v>
+        <v>6.37</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3">
-        <v>6.61</v>
+        <v>6.16</v>
       </c>
       <c r="F33" s="3">
-        <v>2.59</v>
+        <v>14.51</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1751,39 +2136,39 @@
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="E34" s="3">
-        <v>6.59</v>
+        <v>5.3</v>
       </c>
       <c r="F34" s="3">
-        <v>190.88</v>
+        <v>48.34</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>127</v>
+        <v>240</v>
       </c>
       <c r="E35" s="3">
-        <v>6.54</v>
+        <v>4.25</v>
       </c>
       <c r="F35" s="3">
-        <v>2.33</v>
+        <v>13.73</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1791,39 +2176,39 @@
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>96</v>
+        <v>242</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>124</v>
+        <v>243</v>
       </c>
       <c r="E36" s="3">
-        <v>6.5</v>
+        <v>4.93</v>
       </c>
       <c r="F36" s="3">
-        <v>4.8899999999999997</v>
+        <v>28.13</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>125</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="E37" s="3">
-        <v>6.43</v>
+        <v>14.56</v>
       </c>
       <c r="F37" s="3">
-        <v>22</v>
+        <v>3.96</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>165</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -1831,219 +2216,219 @@
         <v>48</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>49</v>
+        <v>163</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="E38" s="3">
-        <v>6.41</v>
+        <v>4.21</v>
       </c>
       <c r="F38" s="3">
-        <v>103.07</v>
+        <v>217.54</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>51</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>80</v>
+        <v>247</v>
       </c>
       <c r="E39" s="3">
-        <v>6.37</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F39" s="3">
-        <v>70.39</v>
+        <v>2.16</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>81</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>168</v>
+        <v>249</v>
       </c>
       <c r="E40" s="3">
-        <v>6.37</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="F40" s="3">
-        <v>207.74</v>
+        <v>12.32</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>169</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="E41" s="3">
-        <v>6.27</v>
+        <v>6.85</v>
       </c>
       <c r="F41" s="3">
-        <v>42.47</v>
+        <v>49.37</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>176</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>46</v>
+        <v>256</v>
       </c>
       <c r="E42" s="3">
-        <v>6.24</v>
+        <v>4.47</v>
       </c>
       <c r="F42" s="3">
-        <v>93.31</v>
+        <v>73.12</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>47</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>142</v>
+        <v>251</v>
       </c>
       <c r="E43" s="3">
-        <v>6.22</v>
+        <v>4.51</v>
       </c>
       <c r="F43" s="3">
-        <v>9.31</v>
+        <v>65.7</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>143</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
       <c r="E44" s="3">
-        <v>6.19</v>
+        <v>4.8</v>
       </c>
       <c r="F44" s="3">
-        <v>12.18</v>
+        <v>4.71</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>67</v>
+        <v>258</v>
       </c>
       <c r="E45" s="3">
-        <v>6.16</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="F45" s="3">
-        <v>13.76</v>
+        <v>19.02</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="E46" s="3">
-        <v>6.07</v>
+        <v>5.93</v>
       </c>
       <c r="F46" s="3">
-        <v>3.07</v>
+        <v>14.36</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="E47" s="3">
-        <v>6.06</v>
+        <v>7.43</v>
       </c>
       <c r="F47" s="3">
-        <v>3.91</v>
+        <v>4.92</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="E48" s="3">
-        <v>6</v>
+        <v>6.31</v>
       </c>
       <c r="F48" s="3">
-        <v>7.29</v>
+        <v>72.17</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
@@ -2057,10 +2442,10 @@
         <v>82</v>
       </c>
       <c r="E49" s="3">
-        <v>5.98</v>
+        <v>6.01</v>
       </c>
       <c r="F49" s="3">
-        <v>24.99</v>
+        <v>24.77</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>83</v>
@@ -2068,182 +2453,182 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>150</v>
+        <v>264</v>
       </c>
       <c r="E50" s="3">
-        <v>5.98</v>
+        <v>4.91</v>
       </c>
       <c r="F50" s="3">
-        <v>118.82</v>
+        <v>35.57</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>151</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>192</v>
+        <v>260</v>
       </c>
       <c r="E51" s="3">
-        <v>5.98</v>
+        <v>4.21</v>
       </c>
       <c r="F51" s="3">
-        <v>116.29</v>
+        <v>2.65</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>193</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E52" s="3">
-        <v>5.94</v>
+        <v>5.16</v>
       </c>
       <c r="F52" s="3">
-        <v>14.42</v>
+        <v>288.77</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="E53" s="3">
-        <v>5.93</v>
+        <v>5.22</v>
       </c>
       <c r="F53" s="3">
-        <v>32.590000000000003</v>
+        <v>2.92</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="E54" s="3">
-        <v>5.89</v>
+        <v>4.07</v>
       </c>
       <c r="F54" s="3">
-        <v>2.63</v>
+        <v>80.12</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>131</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>190</v>
+        <v>268</v>
       </c>
       <c r="E55" s="3">
-        <v>5.82</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="F55" s="3">
-        <v>35.01</v>
+        <v>83.09</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>191</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="E56" s="3">
-        <v>5.76</v>
+        <v>6.82</v>
       </c>
       <c r="F56" s="3">
-        <v>108.73</v>
+        <v>31.27</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="E57" s="3">
-        <v>5.76</v>
+        <v>5.13</v>
       </c>
       <c r="F57" s="3">
-        <v>5.48</v>
+        <v>330.35</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>166</v>
+        <v>271</v>
       </c>
       <c r="E58" s="3">
-        <v>5.74</v>
+        <v>4.47</v>
       </c>
       <c r="F58" s="3">
-        <v>65.77</v>
+        <v>4.74</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>167</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
@@ -2254,56 +2639,56 @@
         <v>17</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>182</v>
+        <v>92</v>
       </c>
       <c r="E59" s="3">
-        <v>5.68</v>
+        <v>9.66</v>
       </c>
       <c r="F59" s="3">
-        <v>44.93</v>
+        <v>2.16</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>183</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>43</v>
+        <v>273</v>
       </c>
       <c r="E60" s="3">
-        <v>5.67</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="F60" s="3">
-        <v>29.83</v>
+        <v>5.33</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>44</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>111</v>
+        <v>275</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>112</v>
+        <v>276</v>
       </c>
       <c r="E61" s="3">
-        <v>5.66</v>
+        <v>4.51</v>
       </c>
       <c r="F61" s="3">
-        <v>4</v>
+        <v>5.3</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>113</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
@@ -2314,256 +2699,256 @@
         <v>17</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>54</v>
+        <v>278</v>
       </c>
       <c r="E62" s="3">
-        <v>5.61</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="F62" s="3">
-        <v>5.01</v>
+        <v>17.95</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>55</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="E63" s="3">
-        <v>5.6</v>
+        <v>7.8</v>
       </c>
       <c r="F63" s="3">
-        <v>53.39</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="E64" s="3">
-        <v>5.47</v>
+        <v>6.03</v>
       </c>
       <c r="F64" s="3">
-        <v>10.55</v>
+        <v>2.7</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E65" s="3">
-        <v>5.46</v>
+        <v>11.98</v>
       </c>
       <c r="F65" s="3">
-        <v>8.68</v>
+        <v>17.61</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>57</v>
+        <v>283</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>159</v>
+        <v>284</v>
       </c>
       <c r="E66" s="3">
-        <v>5.45</v>
+        <v>4.42</v>
       </c>
       <c r="F66" s="3">
-        <v>9.73</v>
+        <v>2.5</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>160</v>
+        <v>285</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>21</v>
+        <v>281</v>
       </c>
       <c r="E67" s="3">
-        <v>5.44</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="F67" s="3">
-        <v>273.87</v>
+        <v>125.02</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>22</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="E68" s="3">
-        <v>5.44</v>
+        <v>6.2</v>
       </c>
       <c r="F68" s="3">
-        <v>41.01</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>6</v>
+        <v>173</v>
       </c>
       <c r="E69" s="3">
-        <v>5.38</v>
+        <v>5.13</v>
       </c>
       <c r="F69" s="3">
-        <v>10.78</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>7</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="E70" s="3">
-        <v>5.33</v>
+        <v>5.17</v>
       </c>
       <c r="F70" s="3">
-        <v>47.74</v>
+        <v>51.08</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="E71" s="3">
-        <v>5.33</v>
+        <v>5.47</v>
       </c>
       <c r="F71" s="3">
-        <v>21.82</v>
+        <v>8.67</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>37</v>
+        <v>286</v>
       </c>
       <c r="E72" s="3">
-        <v>5.31</v>
+        <v>4.96</v>
       </c>
       <c r="F72" s="3">
-        <v>56.99</v>
+        <v>45.82</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>38</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="E73" s="3">
-        <v>5.29</v>
+        <v>5.82</v>
       </c>
       <c r="F73" s="3">
-        <v>30.5</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="E74" s="3">
-        <v>5.26</v>
+        <v>6.76</v>
       </c>
       <c r="F74" s="3">
-        <v>5.0199999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>34</v>
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.2">
@@ -2571,39 +2956,39 @@
         <v>4</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>205</v>
+        <v>288</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>206</v>
+        <v>289</v>
       </c>
       <c r="E75" s="3">
-        <v>5.26</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="F75" s="3">
-        <v>2.86</v>
+        <v>2.1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>207</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E76" s="3">
-        <v>5.22</v>
+        <v>5.99</v>
       </c>
       <c r="F76" s="3">
-        <v>50.88</v>
+        <v>32.869999999999997</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
@@ -2611,99 +2996,99 @@
         <v>16</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="E77" s="3">
-        <v>5.2</v>
+        <v>6.98</v>
       </c>
       <c r="F77" s="3">
-        <v>2.87</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>186</v>
+        <v>120</v>
       </c>
       <c r="E78" s="3">
-        <v>5.2</v>
+        <v>6.51</v>
       </c>
       <c r="F78" s="3">
-        <v>4.96</v>
+        <v>2.59</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>187</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="E79" s="3">
-        <v>5.13</v>
+        <v>7.17</v>
       </c>
       <c r="F79" s="3">
-        <v>329.69</v>
+        <v>14.87</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>172</v>
+        <v>291</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>173</v>
+        <v>292</v>
       </c>
       <c r="E80" s="3">
-        <v>5.13</v>
+        <v>4.13</v>
       </c>
       <c r="F80" s="3">
-        <v>4.57</v>
+        <v>5.17</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>174</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B81" s="3" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>198</v>
+        <v>126</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>199</v>
+        <v>127</v>
       </c>
       <c r="E81" s="3">
-        <v>5.13</v>
+        <v>6.46</v>
       </c>
       <c r="F81" s="3">
-        <v>5.43</v>
+        <v>2.39</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>200</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.2">
@@ -2711,59 +3096,59 @@
         <v>16</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>148</v>
+        <v>294</v>
       </c>
       <c r="E82" s="3">
-        <v>5.0599999999999996</v>
+        <v>4.45</v>
       </c>
       <c r="F82" s="3">
-        <v>3.39</v>
+        <v>2.02</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>149</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B83" s="3" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="E83" s="3">
-        <v>5.05</v>
+        <v>5.86</v>
       </c>
       <c r="F83" s="3">
-        <v>282.20999999999998</v>
+        <v>2.65</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="E84" s="3">
-        <v>5.04</v>
+        <v>6.09</v>
       </c>
       <c r="F84" s="3">
-        <v>9.82</v>
+        <v>7.49</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.2">
@@ -2771,24 +3156,1124 @@
         <v>16</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E85" s="3">
+        <v>7.47</v>
+      </c>
+      <c r="F85" s="3">
+        <v>3.35</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E86" s="3">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F86" s="3">
+        <v>2.97</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E87" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="F87" s="3">
+        <v>3.53</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="E88" s="3">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="F88" s="3">
+        <v>12.05</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B89" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E89" s="3">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F89" s="3">
+        <v>11.83</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E90" s="3">
+        <v>4.28</v>
+      </c>
+      <c r="F90" s="3">
+        <v>33.64</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B91" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E91" s="3">
+        <v>4.01</v>
+      </c>
+      <c r="F91" s="3">
+        <v>3.75</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B92" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E92" s="3">
+        <v>5.29</v>
+      </c>
+      <c r="F92" s="3">
+        <v>30.29</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B93" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E93" s="3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="F93" s="3">
+        <v>23.63</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B94" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D94" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E94" s="3">
+        <v>6.76</v>
+      </c>
+      <c r="F94" s="3">
+        <v>2.64</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E95" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="F95" s="3">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B96" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E96" s="3">
+        <v>8.34</v>
+      </c>
+      <c r="F96" s="3">
+        <v>24.85</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B97" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E97" s="3">
+        <v>5.13</v>
+      </c>
+      <c r="F97" s="3">
+        <v>3.48</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E98" s="3">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="F98" s="3">
+        <v>6.11</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B99" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E99" s="3">
+        <v>4.03</v>
+      </c>
+      <c r="F99" s="3">
+        <v>197.96</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E100" s="3">
+        <v>6.04</v>
+      </c>
+      <c r="F100" s="3">
+        <v>120.97</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B101" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E101" s="3">
+        <v>5.44</v>
+      </c>
+      <c r="F101" s="3">
+        <v>22.07</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E102" s="3">
+        <v>4.13</v>
+      </c>
+      <c r="F102" s="3">
+        <v>15.04</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B103" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E103" s="3">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F103" s="3">
+        <v>35.24</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B104" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E104" s="3">
+        <v>4.99</v>
+      </c>
+      <c r="F104" s="3">
+        <v>8.74</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E105" s="3">
+        <v>7.73</v>
+      </c>
+      <c r="F105" s="3">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B106" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E106" s="3">
+        <v>5.45</v>
+      </c>
+      <c r="F106" s="3">
+        <v>9.68</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B107" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E107" s="3">
+        <v>6.99</v>
+      </c>
+      <c r="F107" s="3">
+        <v>15.12</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B108" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E108" s="3">
+        <v>6.43</v>
+      </c>
+      <c r="F108" s="3">
+        <v>22.77</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B109" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E109" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="F109" s="3">
+        <v>67.09</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B110" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" s="3">
+        <v>6.47</v>
+      </c>
+      <c r="F110" s="3">
+        <v>211.6</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B111" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E111" s="3">
+        <v>12.66</v>
+      </c>
+      <c r="F111" s="3">
+        <v>2.04</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B112" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E112" s="3">
+        <v>6.47</v>
+      </c>
+      <c r="F112" s="3">
+        <v>42.97</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B113" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E113" s="3">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F113" s="3">
+        <v>6.81</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E114" s="3">
+        <v>6.43</v>
+      </c>
+      <c r="F114" s="3">
+        <v>2.17</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B115" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E115" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="F115" s="3">
+        <v>45.34</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E116" s="3">
+        <v>6.41</v>
+      </c>
+      <c r="F116" s="3">
+        <v>196.74</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B117" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E117" s="3">
+        <v>9.17</v>
+      </c>
+      <c r="F117" s="3">
+        <v>20.55</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B118" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E118" s="3">
+        <v>4.04</v>
+      </c>
+      <c r="F118" s="3">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B119" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E119" s="3">
+        <v>7.84</v>
+      </c>
+      <c r="F119" s="3">
+        <v>13</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E120" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="F120" s="3">
+        <v>5.09</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B121" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E121" s="3">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F121" s="3">
+        <v>6.64</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B122" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E122" s="3">
+        <v>4.87</v>
+      </c>
+      <c r="F122" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B123" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E123" s="3">
+        <v>4.34</v>
+      </c>
+      <c r="F123" s="3">
+        <v>45.88</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B124" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E124" s="3">
+        <v>4.22</v>
+      </c>
+      <c r="F124" s="3">
+        <v>3.22</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B125" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E125" s="3">
+        <v>5.87</v>
+      </c>
+      <c r="F125" s="3">
+        <v>35.61</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B126" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E126" s="3">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="F126" s="3">
+        <v>132.9</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B127" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E127" s="3">
+        <v>5.87</v>
+      </c>
+      <c r="F127" s="3">
+        <v>120.66</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E128" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="F128" s="3">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B129" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E129" s="3">
+        <v>5.21</v>
+      </c>
+      <c r="F129" s="3">
+        <v>5.44</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B130" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E130" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="F130" s="3">
+        <v>35.56</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B131" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E131" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="F131" s="3">
+        <v>27.25</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B132" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E132" s="3">
+        <v>5.64</v>
+      </c>
+      <c r="F132" s="3">
+        <v>10.41</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B133" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E133" s="3">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F133" s="3">
+        <v>247.44</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B134" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D134" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E134" s="3">
         <v>5.03</v>
       </c>
-      <c r="F85" s="3">
-        <v>43.28</v>
-      </c>
-      <c r="G85" s="3" t="s">
+      <c r="F134" s="3">
+        <v>43.54</v>
+      </c>
+      <c r="G134" s="3" t="s">
         <v>202</v>
       </c>
     </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B135" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E135" s="3">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="F135" s="3">
+        <v>15.57</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B136" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E136" s="3">
+        <v>4.24</v>
+      </c>
+      <c r="F136" s="3">
+        <v>214.36</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B137" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E137" s="3">
+        <v>8.25</v>
+      </c>
+      <c r="F137" s="3">
+        <v>18.23</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B138" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E138" s="3">
+        <v>6.21</v>
+      </c>
+      <c r="F138" s="3">
+        <v>11.66</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B139" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E139" s="3">
+        <v>5.27</v>
+      </c>
+      <c r="F139" s="3">
+        <v>2.86</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B140" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E140" s="3">
+        <v>6.46</v>
+      </c>
+      <c r="F140" s="3">
+        <v>29.36</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B3:G85">
-    <sortCondition descending="1" ref="E3:E85"/>
+  <sortState ref="B3:G140">
+    <sortCondition ref="D2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Optimizado el funcionamiento en la búsqueda de URLs a partir del nombre de la empresa
</commit_message>
<xml_diff>
--- a/Screenshots/_Screenshots.xlsx
+++ b/Screenshots/_Screenshots.xlsx
@@ -7,15 +7,22 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="28380" windowHeight="12915"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos Screenshots" sheetId="1" r:id="rId1"/>
+    <sheet name="DCWebUrlFromNombreEmpresa" sheetId="1" r:id="rId1"/>
+    <sheet name="DCChartFromWebUrl" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Screenshots" localSheetId="0">'Datos Screenshots'!$B$3:$AR$133</definedName>
-    <definedName name="_Screenshots_1" localSheetId="0">'Datos Screenshots'!#REF!</definedName>
-    <definedName name="_Screenshots_2" localSheetId="0">'Datos Screenshots'!#REF!</definedName>
-    <definedName name="header" localSheetId="0">'Datos Screenshots'!#REF!</definedName>
-    <definedName name="new_1" localSheetId="0">'Datos Screenshots'!#REF!</definedName>
-    <definedName name="tmp" localSheetId="0">'Datos Screenshots'!#REF!</definedName>
+    <definedName name="_Screenshots" localSheetId="1">DCChartFromWebUrl!$B$3:$AR$133</definedName>
+    <definedName name="_Screenshots" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
+    <definedName name="_Screenshots_1" localSheetId="1">DCChartFromWebUrl!#REF!</definedName>
+    <definedName name="_Screenshots_1" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
+    <definedName name="_Screenshots_2" localSheetId="1">DCChartFromWebUrl!#REF!</definedName>
+    <definedName name="_Screenshots_2" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
+    <definedName name="header" localSheetId="1">DCChartFromWebUrl!#REF!</definedName>
+    <definedName name="header" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
+    <definedName name="new_1" localSheetId="1">DCChartFromWebUrl!#REF!</definedName>
+    <definedName name="new_1" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
+    <definedName name="tmp" localSheetId="1">DCChartFromWebUrl!#REF!</definedName>
+    <definedName name="tmp" localSheetId="0">DCWebUrlFromNombreEmpresa!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -322,47 +329,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="header" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\header.txt" decimal="," thousands="." tab="0" semicolon="1">
-      <textFields count="81">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="7" name="_Screenshots41" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\_PELAYO\Software\Eclipse Neon\workspace\markets_data\Screenshots\_Screenshots.txt" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="43">
         <textField/>
         <textField/>
         <textField/>
@@ -409,7 +378,94 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="new 1" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="8" name="header" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\header.txt" decimal="," thousands="." tab="0" semicolon="1">
+      <textFields count="81">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="new 1" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\new 1.txt" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="6">
         <textField type="text"/>
@@ -421,7 +477,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="tmp" type="6" refreshedVersion="4" background="1" saveData="1">
+  <connection id="10" name="tmp" type="6" refreshedVersion="4" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\Empleado\Desktop\tmp.txt" decimal="," thousands="." tab="0" semicolon="1">
       <textFields count="6">
         <textField/>
@@ -437,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="373">
   <si>
     <t>Sector</t>
   </si>
@@ -1605,6 +1661,25 @@
   </si>
   <si>
     <t>https://es.investing.com/equities/suncor-energy-inc.</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>URL Investing</t>
+  </si>
+  <si>
+    <t>Magnitud 
+Capitalización</t>
+  </si>
+  <si>
+    <t>Capitalización</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1790,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="_Screenshots" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="_Screenshots" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2005,9 +2080,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="58.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="22.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B3:AR133">
+    <sortCondition ref="D3:D133"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AR133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -19357,9 +19485,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:AR133">
-    <sortCondition ref="D3:D133"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>